<commit_message>
Added fact fruit, test antioxidant
</commit_message>
<xml_diff>
--- a/foodSamples.xlsx
+++ b/foodSamples.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Asked" sheetId="4" r:id="rId3"/>
+    <sheet name="AntiOx" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="218">
   <si>
     <t>food_name: "brocolli",</t>
   </si>
@@ -501,54 +502,6 @@
     <t>nf_potassium: 108.1,</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Brocolli</t>
-  </si>
-  <si>
-    <t>Serving gram</t>
-  </si>
-  <si>
-    <t>Total gm</t>
-  </si>
-  <si>
-    <t>Calories</t>
-  </si>
-  <si>
-    <t>Total Fat</t>
-  </si>
-  <si>
-    <t>S Fat</t>
-  </si>
-  <si>
-    <t>Cholestrol</t>
-  </si>
-  <si>
-    <t>Sodium</t>
-  </si>
-  <si>
-    <t>Carbs</t>
-  </si>
-  <si>
-    <t>Fiber</t>
-  </si>
-  <si>
-    <t>Sugar</t>
-  </si>
-  <si>
-    <t>Protien</t>
-  </si>
-  <si>
-    <t>Potass</t>
-  </si>
-  <si>
-    <t>Phos</t>
-  </si>
-  <si>
-    <t>Quinua Salad</t>
-  </si>
-  <si>
     <t>ALC</t>
   </si>
   <si>
@@ -640,13 +593,91 @@
   </si>
   <si>
     <t>Folic acid</t>
+  </si>
+  <si>
+    <t>Yogurt</t>
+  </si>
+  <si>
+    <t>Bannana</t>
+  </si>
+  <si>
+    <t>Avocado</t>
+  </si>
+  <si>
+    <t>Mushroom</t>
+  </si>
+  <si>
+    <t>Sade Paneer</t>
+  </si>
+  <si>
+    <t>Soilent</t>
+  </si>
+  <si>
+    <t>Amber Night</t>
+  </si>
+  <si>
+    <t>Jasmine Rice</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>Biryani</t>
+  </si>
+  <si>
+    <t>Oats</t>
+  </si>
+  <si>
+    <t>Strawberries</t>
+  </si>
+  <si>
+    <t>LYCPN</t>
+  </si>
+  <si>
+    <t>Lycopene</t>
+  </si>
+  <si>
+    <t>Raw Value</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Total Grams</t>
+  </si>
+  <si>
+    <t>Papaya</t>
+  </si>
+  <si>
+    <t>Carotene</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>VitC</t>
+  </si>
+  <si>
+    <t>VitE</t>
+  </si>
+  <si>
+    <t>green tea</t>
+  </si>
+  <si>
+    <t>green tea 0 0.00735 0 0 0</t>
+  </si>
+  <si>
+    <t>green tea 0 0.30 0 0 0 99 246.20396230000003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,8 +691,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,12 +709,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -698,18 +743,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1734,173 +1857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K1" t="s">
-        <v>172</v>
-      </c>
-      <c r="L1" t="s">
-        <v>173</v>
-      </c>
-      <c r="M1" t="s">
-        <v>174</v>
-      </c>
-      <c r="N1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2">
-        <v>37</v>
-      </c>
-      <c r="C2">
-        <f>SUM(E2,F2,G2,H2,I2,J2,K2,L2,M2,N2)</f>
-        <v>5.5969999999999995</v>
-      </c>
-      <c r="D2">
-        <v>12.95</v>
-      </c>
-      <c r="E2">
-        <v>0.15</v>
-      </c>
-      <c r="F2">
-        <v>0.03</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="I2">
-        <v>2.66</v>
-      </c>
-      <c r="J2">
-        <v>1.22</v>
-      </c>
-      <c r="K2">
-        <v>0.51</v>
-      </c>
-      <c r="L2">
-        <v>0.88</v>
-      </c>
-      <c r="M2">
-        <v>0.108</v>
-      </c>
-      <c r="N2">
-        <v>2.4E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="E3">
-        <f>(E2/C2)*100</f>
-        <v>2.6800071466857247</v>
-      </c>
-      <c r="F3">
-        <f>(F2/C2)*100</f>
-        <v>0.5360014293371449</v>
-      </c>
-      <c r="G3">
-        <f>(G2/C2)*100</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f>(H2/C2)*100</f>
-        <v>0.26800071466857245</v>
-      </c>
-      <c r="I3" s="1">
-        <f>(I2/C2)*100</f>
-        <v>47.525460067893519</v>
-      </c>
-      <c r="J3" s="1">
-        <f>(J2/C2)*100</f>
-        <v>21.79739145971056</v>
-      </c>
-      <c r="K3">
-        <f>(K2/C2)*100</f>
-        <v>9.1120242987314644</v>
-      </c>
-      <c r="L3" s="1">
-        <f>(L2/C2)*100</f>
-        <v>15.722708593889584</v>
-      </c>
-      <c r="M3">
-        <f>(M2/C2)*100</f>
-        <v>1.9296051456137215</v>
-      </c>
-      <c r="N3">
-        <f>(N2/C2)*100</f>
-        <v>0.42880114346971598</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5">
-        <v>239</v>
-      </c>
-      <c r="D5">
-        <v>271.20999999999998</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="21.75" customHeight="1"/>
@@ -1910,203 +1870,608 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A1" s="2">
+      <c r="A1" s="1">
         <v>221</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A2" s="1">
+        <v>255</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A3" s="1">
+        <v>262</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A4" s="1">
+        <v>301</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A5" s="1">
+        <v>303</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A6" s="1">
+        <v>328</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="32.25" thickBot="1">
+      <c r="A7" s="1">
+        <v>401</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A8" s="1">
+        <v>415</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A2" s="2">
-        <v>255</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A9" s="1">
+        <v>418</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A3" s="2">
-        <v>262</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A10" s="1">
+        <v>430</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A11" s="1">
+        <v>317</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="2">
-        <v>301</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A12" s="1">
+        <v>323</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A5" s="2">
-        <v>303</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A13" s="1">
+        <v>321</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="32.25" thickBot="1">
-      <c r="A6" s="2">
-        <v>328</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D13" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A14" s="1">
+        <v>431</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="32.25" thickBot="1">
-      <c r="A7" s="2">
-        <v>401</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A8" s="2">
-        <v>415</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A9" s="2">
-        <v>418</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" thickBot="1">
-      <c r="A10" s="2">
-        <v>430</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A11" s="2">
-        <v>317</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A12" s="2">
-        <v>323</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A13" s="2">
-        <v>321</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="D14" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A15" s="1">
+        <v>337</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A14" s="2">
-        <v>431</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>190</v>
+      <c r="D15" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>43019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>43019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>43019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>43019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>43020</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43060</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>43060</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3">
+        <v>43060</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="B1" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2">
+        <v>247.345</v>
+      </c>
+      <c r="C2" s="7">
+        <v>3.97</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="F2" s="8">
+        <v>52</v>
+      </c>
+      <c r="N2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="C3" s="7">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="D3" s="7">
+        <v>36</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="C4" s="7">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="C5" s="7">
+        <v>26.5</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="C6" s="7">
+        <v>4.3499999999999997E-3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7">
+        <v>237.614</v>
+      </c>
+      <c r="C7">
+        <v>1.218</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>211</v>
+      </c>
+      <c r="F7" s="8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="C8">
+        <v>0.82740000000000002</v>
+      </c>
+      <c r="D8">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="C11">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12">
+        <v>246.2039</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>211</v>
+      </c>
+      <c r="F12" s="11">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="D13">
+        <v>0.3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>212</v>
+      </c>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>214</v>
+      </c>
+      <c r="F16" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="F12:F16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>